<commit_message>
Add final video demo impl
</commit_message>
<xml_diff>
--- a/CIS5-tasks-sheet.xlsx
+++ b/CIS5-tasks-sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Docker" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
   <si>
     <t>NOTES</t>
   </si>
@@ -402,6 +402,12 @@
   <si>
     <t>Found but not implemented in code</t>
   </si>
+  <si>
+    <t>Do not run ssh within containers (Scored)</t>
+  </si>
+  <si>
+    <t>check ssh from proc/{pid}/cmdline</t>
+  </si>
 </sst>
 </file>
 
@@ -410,7 +416,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Done&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +499,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF07181B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -553,7 +567,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -589,8 +603,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -651,16 +677,23 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Bad" xfId="7" builtinId="27"/>
     <cellStyle name="Date" xfId="5"/>
     <cellStyle name="Done" xfId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="4" builtinId="5" customBuiltin="1"/>
@@ -768,8 +801,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tasks4" displayName="Tasks4" ref="B2:E24" totalsRowShown="0" headerRowDxfId="1" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B2:E24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tasks4" displayName="Tasks4" ref="B2:E25" totalsRowShown="0" headerRowDxfId="2" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:E25"/>
   <tableColumns count="4">
     <tableColumn id="1" name="BENCHMARK" dataCellStyle="Table Text"/>
     <tableColumn id="4" name="DEFINITION" dataCellStyle="Date"/>
@@ -786,8 +819,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="B2:E21" totalsRowShown="0" headerRowDxfId="2" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B2:E21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="B2:E22" totalsRowShown="0" headerRowDxfId="1" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:E22"/>
   <tableColumns count="4">
     <tableColumn id="1" name="BENCHMARK" dataCellStyle="Table Text"/>
     <tableColumn id="4" name="DEFINITION" dataCellStyle="Date"/>
@@ -804,8 +837,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tasks3" displayName="Tasks3" ref="B2:E18" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B2:E18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tasks3" displayName="Tasks3" ref="B2:E19" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B2:E19"/>
   <tableColumns count="4">
     <tableColumn id="1" name="BENCHMARK" dataCellStyle="Table Text"/>
     <tableColumn id="4" name="DEFINITION" dataCellStyle="Date"/>
@@ -1028,10 +1061,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E24"/>
+  <dimension ref="B1:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1127,208 +1160,220 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="8">
+      <c r="B8" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8">
         <v>5.7</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="5">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="5">
         <v>5.8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="8">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8">
         <v>5.9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="5">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5">
         <v>5.14</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="8">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="8">
         <v>5.15</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="5">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="5">
         <v>5.16</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="8">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="8">
         <v>5.17</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="5">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="5">
         <v>5.18</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="12" t="s">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="s">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E25" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
@@ -1350,10 +1395,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E25"/>
+  <dimension ref="B1:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="118" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1449,23 +1494,23 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="8">
+      <c r="B8" s="20">
+        <v>5.6</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8">
         <v>5.7</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="5">
-        <v>5.8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>70</v>
@@ -1473,162 +1518,174 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="15">
+      <c r="B10" s="5">
+        <v>5.8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="15">
         <v>5.9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="15">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="15">
         <v>5.15</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="18">
+    <row r="17" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="18">
         <v>5.16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="8">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="8">
         <v>5.17</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="18" t="s">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="24" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="16"/>
-      <c r="C24" t="s">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="25" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="16"/>
+      <c r="C25" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="19"/>
-      <c r="C25" t="s">
+    <row r="26" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="19"/>
+      <c r="C26" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1648,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E21"/>
+  <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1747,147 +1804,159 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="20">
+        <v>5.6</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="8">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8">
         <v>5.15</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="5">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="5">
         <v>5.16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="8">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="8">
         <v>5.17</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="15" t="s">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C18" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="2:5" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="2:5" ht="84" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="16"/>
-      <c r="C20" t="s">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="16"/>
+      <c r="C21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="19"/>
-      <c r="C21" t="s">
+    <row r="22" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="19"/>
+      <c r="C22" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>